<commit_message>
Nov 1st push - Updated 2020 mortality datasets; Pneumonia & Influenza added to CCB Cause List; year parameter added; New url parameter tab
</commit_message>
<xml_diff>
--- a/myCCB/myInfo/queryParameter_Linkage.xlsx
+++ b/myCCB/myInfo/queryParameter_Linkage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB.Jaspo\myCCB\myInfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\myInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E6411B-52CF-4AC0-8C35-D49681EB8839}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA1A87C-4311-44D0-BD7E-79EB5798BC66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{D3A4EB56-BD7B-4DE5-B361-4DC1FFA4D382}"/>
+    <workbookView xWindow="0" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{D3A4EB56-BD7B-4DE5-B361-4DC1FFA4D382}"/>
   </bookViews>
   <sheets>
     <sheet name="tab" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="370">
   <si>
     <t>ccbName</t>
   </si>
@@ -1077,9 +1077,6 @@
     <t>hospitalPrimaryAnyTab</t>
   </si>
   <si>
-    <t>abouts</t>
-  </si>
-  <si>
     <t>overviewTab</t>
   </si>
   <si>
@@ -1138,6 +1135,18 @@
   </si>
   <si>
     <t>otherlinks</t>
+  </si>
+  <si>
+    <t>about</t>
+  </si>
+  <si>
+    <t>CCB URL PARAMETERS</t>
+  </si>
+  <si>
+    <t>urlParametersTab</t>
+  </si>
+  <si>
+    <t>urlparameters</t>
   </si>
 </sst>
 </file>
@@ -1489,10 +1498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F50DBCD-5A3C-4AED-A7E8-75EA46ECE524}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,7 +1549,7 @@
         <v>340</v>
       </c>
       <c r="E3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1557,7 +1566,7 @@
         <v>333</v>
       </c>
       <c r="E4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1574,7 +1583,7 @@
         <v>334</v>
       </c>
       <c r="E5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1591,7 +1600,7 @@
         <v>335</v>
       </c>
       <c r="E6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1608,7 +1617,7 @@
         <v>336</v>
       </c>
       <c r="E7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1625,7 +1634,7 @@
         <v>337</v>
       </c>
       <c r="E8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1642,7 +1651,7 @@
         <v>338</v>
       </c>
       <c r="E9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1659,7 +1668,7 @@
         <v>327</v>
       </c>
       <c r="E10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1676,7 +1685,7 @@
         <v>328</v>
       </c>
       <c r="E11" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1693,7 +1702,7 @@
         <v>329</v>
       </c>
       <c r="E12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1710,7 +1719,7 @@
         <v>330</v>
       </c>
       <c r="E13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1727,7 +1736,7 @@
         <v>331</v>
       </c>
       <c r="E14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1778,7 +1787,7 @@
         <v>344</v>
       </c>
       <c r="E17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1795,7 +1804,7 @@
         <v>345</v>
       </c>
       <c r="E18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1828,13 +1837,13 @@
         <v>319</v>
       </c>
       <c r="C21" t="s">
+        <v>366</v>
+      </c>
+      <c r="D21" t="s">
         <v>346</v>
       </c>
-      <c r="D21" t="s">
-        <v>347</v>
-      </c>
       <c r="E21" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1845,13 +1854,13 @@
         <v>320</v>
       </c>
       <c r="C22" t="s">
-        <v>346</v>
+        <v>366</v>
       </c>
       <c r="D22" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E22" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1862,13 +1871,30 @@
         <v>321</v>
       </c>
       <c r="C23" t="s">
-        <v>346</v>
+        <v>366</v>
       </c>
       <c r="D23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E23" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>303</v>
+      </c>
+      <c r="B24" t="s">
+        <v>367</v>
+      </c>
+      <c r="C24" t="s">
         <v>366</v>
+      </c>
+      <c r="D24" t="s">
+        <v>368</v>
+      </c>
+      <c r="E24" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add broad condition error note, and new tab to parameter list for hyperlinking
</commit_message>
<xml_diff>
--- a/myCCB/myInfo/queryParameter_Linkage.xlsx
+++ b/myCCB/myInfo/queryParameter_Linkage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\myInfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB.Jaspo\myCCB\myInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA1A87C-4311-44D0-BD7E-79EB5798BC66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92982C4-1125-4FDF-90C8-79ACE934C0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{D3A4EB56-BD7B-4DE5-B361-4DC1FFA4D382}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{D3A4EB56-BD7B-4DE5-B361-4DC1FFA4D382}"/>
   </bookViews>
   <sheets>
     <sheet name="tab" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="373">
   <si>
     <t>ccbName</t>
   </si>
@@ -1147,6 +1147,15 @@
   </si>
   <si>
     <t>urlparameters</t>
+  </si>
+  <si>
+    <t>LEADING CAUSES TREND</t>
+  </si>
+  <si>
+    <t>topTrendsTab</t>
+  </si>
+  <si>
+    <t>leadingcausestrend</t>
   </si>
 </sst>
 </file>
@@ -1498,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F50DBCD-5A3C-4AED-A7E8-75EA46ECE524}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,53 +1750,53 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B15" t="s">
-        <v>298</v>
+        <v>370</v>
       </c>
       <c r="C15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D15" t="s">
-        <v>341</v>
+        <v>371</v>
       </c>
       <c r="E15" t="s">
-        <v>323</v>
+        <v>372</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B16" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="C16" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D16" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E16" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D17" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E17" t="s">
-        <v>358</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1795,55 +1804,55 @@
         <v>300</v>
       </c>
       <c r="B18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C18" t="s">
         <v>325</v>
       </c>
       <c r="D18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B19" t="s">
-        <v>301</v>
+        <v>318</v>
       </c>
       <c r="C19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D19" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="E19" t="s">
-        <v>326</v>
+        <v>359</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>302</v>
+        <v>301</v>
+      </c>
+      <c r="B20" t="s">
+        <v>301</v>
+      </c>
+      <c r="C20" t="s">
+        <v>326</v>
+      </c>
+      <c r="D20" t="s">
+        <v>343</v>
+      </c>
+      <c r="E20" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>303</v>
-      </c>
-      <c r="B21" t="s">
-        <v>319</v>
-      </c>
-      <c r="C21" t="s">
-        <v>366</v>
-      </c>
-      <c r="D21" t="s">
-        <v>346</v>
-      </c>
-      <c r="E21" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1851,16 +1860,16 @@
         <v>303</v>
       </c>
       <c r="B22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C22" t="s">
         <v>366</v>
       </c>
       <c r="D22" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E22" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1868,16 +1877,16 @@
         <v>303</v>
       </c>
       <c r="B23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C23" t="s">
         <v>366</v>
       </c>
       <c r="D23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E23" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1885,15 +1894,32 @@
         <v>303</v>
       </c>
       <c r="B24" t="s">
-        <v>367</v>
+        <v>321</v>
       </c>
       <c r="C24" t="s">
         <v>366</v>
       </c>
       <c r="D24" t="s">
+        <v>348</v>
+      </c>
+      <c r="E24" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>303</v>
+      </c>
+      <c r="B25" t="s">
+        <v>367</v>
+      </c>
+      <c r="C25" t="s">
+        <v>366</v>
+      </c>
+      <c r="D25" t="s">
         <v>368</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>369</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove injury suppression; Add url for multiple lenses; updates and injury modal
</commit_message>
<xml_diff>
--- a/myCCB/myInfo/queryParameter_Linkage.xlsx
+++ b/myCCB/myInfo/queryParameter_Linkage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\myInfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB.dev\myCCB\myInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEFA122-7FF0-44D1-9F2B-16F393AC1248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264C8E45-4148-4A6A-ACD2-C5552C37EAB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{D3A4EB56-BD7B-4DE5-B361-4DC1FFA4D382}"/>
+    <workbookView xWindow="7815" yWindow="5505" windowWidth="21600" windowHeight="13215" xr2:uid="{D3A4EB56-BD7B-4DE5-B361-4DC1FFA4D382}"/>
   </bookViews>
   <sheets>
     <sheet name="tab" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="387">
   <si>
     <t>ccbName</t>
   </si>
@@ -1165,6 +1165,39 @@
   </si>
   <si>
     <t>MULTIPLE CAUSES OF DEATH</t>
+  </si>
+  <si>
+    <t>MULTIPLE LENSES</t>
+  </si>
+  <si>
+    <t>MORTALITY</t>
+  </si>
+  <si>
+    <t>MORBIDITY</t>
+  </si>
+  <si>
+    <t>YLD AND RISK</t>
+  </si>
+  <si>
+    <t>multipleLenses</t>
+  </si>
+  <si>
+    <t>causeOfDeathTab</t>
+  </si>
+  <si>
+    <t>nonFatalMeasuresTab</t>
+  </si>
+  <si>
+    <t>stateMeasuresTab</t>
+  </si>
+  <si>
+    <t>mortalitylens</t>
+  </si>
+  <si>
+    <t>morbiditylens</t>
+  </si>
+  <si>
+    <t>risklens</t>
   </si>
 </sst>
 </file>
@@ -1516,10 +1549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F50DBCD-5A3C-4AED-A7E8-75EA46ECE524}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,143 +1826,143 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>298</v>
+        <v>376</v>
       </c>
       <c r="B17" t="s">
-        <v>298</v>
+        <v>377</v>
       </c>
       <c r="C17" t="s">
-        <v>323</v>
+        <v>380</v>
       </c>
       <c r="D17" t="s">
-        <v>341</v>
+        <v>381</v>
       </c>
       <c r="E17" t="s">
-        <v>323</v>
+        <v>384</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>299</v>
+        <v>376</v>
       </c>
       <c r="B18" t="s">
-        <v>316</v>
+        <v>378</v>
       </c>
       <c r="C18" t="s">
-        <v>324</v>
+        <v>380</v>
       </c>
       <c r="D18" t="s">
-        <v>342</v>
+        <v>382</v>
       </c>
       <c r="E18" t="s">
-        <v>324</v>
+        <v>385</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>300</v>
+        <v>376</v>
       </c>
       <c r="B19" t="s">
-        <v>317</v>
+        <v>379</v>
       </c>
       <c r="C19" t="s">
-        <v>325</v>
+        <v>380</v>
       </c>
       <c r="D19" t="s">
-        <v>344</v>
+        <v>383</v>
       </c>
       <c r="E19" t="s">
-        <v>358</v>
+        <v>386</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B20" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="C20" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D20" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E20" t="s">
-        <v>359</v>
+        <v>323</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B21" t="s">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="C21" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D21" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E21" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>302</v>
+        <v>300</v>
+      </c>
+      <c r="B22" t="s">
+        <v>317</v>
+      </c>
+      <c r="C22" t="s">
+        <v>325</v>
+      </c>
+      <c r="D22" t="s">
+        <v>344</v>
+      </c>
+      <c r="E22" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C23" t="s">
-        <v>366</v>
+        <v>325</v>
       </c>
       <c r="D23" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E23" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B24" t="s">
-        <v>320</v>
+        <v>301</v>
       </c>
       <c r="C24" t="s">
-        <v>366</v>
+        <v>326</v>
       </c>
       <c r="D24" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E24" t="s">
-        <v>364</v>
+        <v>326</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>303</v>
-      </c>
-      <c r="B25" t="s">
-        <v>321</v>
-      </c>
-      <c r="C25" t="s">
-        <v>366</v>
-      </c>
-      <c r="D25" t="s">
-        <v>348</v>
-      </c>
-      <c r="E25" t="s">
-        <v>365</v>
+        <v>302</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1937,15 +1970,66 @@
         <v>303</v>
       </c>
       <c r="B26" t="s">
-        <v>367</v>
+        <v>319</v>
       </c>
       <c r="C26" t="s">
         <v>366</v>
       </c>
       <c r="D26" t="s">
+        <v>346</v>
+      </c>
+      <c r="E26" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>303</v>
+      </c>
+      <c r="B27" t="s">
+        <v>320</v>
+      </c>
+      <c r="C27" t="s">
+        <v>366</v>
+      </c>
+      <c r="D27" t="s">
+        <v>347</v>
+      </c>
+      <c r="E27" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>303</v>
+      </c>
+      <c r="B28" t="s">
+        <v>321</v>
+      </c>
+      <c r="C28" t="s">
+        <v>366</v>
+      </c>
+      <c r="D28" t="s">
+        <v>348</v>
+      </c>
+      <c r="E28" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>303</v>
+      </c>
+      <c r="B29" t="s">
+        <v>367</v>
+      </c>
+      <c r="C29" t="s">
+        <v>366</v>
+      </c>
+      <c r="D29" t="s">
         <v>368</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E29" t="s">
         <v>369</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refine IHME tab in CCB; Clean up IHME files
</commit_message>
<xml_diff>
--- a/myCCB/myInfo/queryParameter_Linkage.xlsx
+++ b/myCCB/myInfo/queryParameter_Linkage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\myInfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB.dev\myCCB\myInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2115DC-9617-4429-9175-48A95A9DD4B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD127ED-DED4-45CA-B401-023E1D0A588F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="3300" windowWidth="27990" windowHeight="15435" xr2:uid="{D3A4EB56-BD7B-4DE5-B361-4DC1FFA4D382}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D3A4EB56-BD7B-4DE5-B361-4DC1FFA4D382}"/>
   </bookViews>
   <sheets>
     <sheet name="tab" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="393">
   <si>
     <t>ccbName</t>
   </si>
@@ -1125,9 +1125,6 @@
     <t>deathhosped</t>
   </si>
   <si>
-    <t>risksihme</t>
-  </si>
-  <si>
     <t>ihmerankings</t>
   </si>
   <si>
@@ -1207,6 +1204,18 @@
   </si>
   <si>
     <t>lifecourse</t>
+  </si>
+  <si>
+    <t>IHME</t>
+  </si>
+  <si>
+    <t>ihmeTab</t>
+  </si>
+  <si>
+    <t>risksihmeARCHIVED</t>
+  </si>
+  <si>
+    <t>ihmerankingsARCHIVED</t>
   </si>
 </sst>
 </file>
@@ -1558,10 +1567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F50DBCD-5A3C-4AED-A7E8-75EA46ECE524}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,7 +1579,7 @@
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1651,16 +1660,16 @@
         <v>296</v>
       </c>
       <c r="B6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C6" t="s">
         <v>332</v>
       </c>
       <c r="D6" t="s">
+        <v>387</v>
+      </c>
+      <c r="E6" t="s">
         <v>388</v>
-      </c>
-      <c r="E6" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1668,16 +1677,16 @@
         <v>296</v>
       </c>
       <c r="B7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C7" t="s">
         <v>332</v>
       </c>
       <c r="D7" t="s">
+        <v>372</v>
+      </c>
+      <c r="E7" t="s">
         <v>373</v>
-      </c>
-      <c r="E7" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1728,7 +1737,7 @@
         <v>337</v>
       </c>
       <c r="E10" t="s">
-        <v>362</v>
+        <v>391</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1745,24 +1754,24 @@
         <v>338</v>
       </c>
       <c r="E11" t="s">
-        <v>363</v>
+        <v>392</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B12" t="s">
-        <v>311</v>
+        <v>389</v>
       </c>
       <c r="C12" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="D12" t="s">
-        <v>327</v>
+        <v>390</v>
       </c>
       <c r="E12" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1770,16 +1779,16 @@
         <v>297</v>
       </c>
       <c r="B13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C13" t="s">
         <v>322</v>
       </c>
       <c r="D13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1787,16 +1796,16 @@
         <v>297</v>
       </c>
       <c r="B14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C14" t="s">
         <v>322</v>
       </c>
       <c r="D14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1804,16 +1813,16 @@
         <v>297</v>
       </c>
       <c r="B15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C15" t="s">
         <v>322</v>
       </c>
       <c r="D15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E15" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1821,16 +1830,16 @@
         <v>297</v>
       </c>
       <c r="B16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C16" t="s">
         <v>322</v>
       </c>
       <c r="D16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E16" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1838,118 +1847,118 @@
         <v>297</v>
       </c>
       <c r="B17" t="s">
-        <v>370</v>
+        <v>315</v>
       </c>
       <c r="C17" t="s">
         <v>322</v>
       </c>
       <c r="D17" t="s">
-        <v>371</v>
+        <v>331</v>
       </c>
       <c r="E17" t="s">
-        <v>372</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>376</v>
+        <v>297</v>
       </c>
       <c r="B18" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C18" t="s">
-        <v>380</v>
+        <v>322</v>
       </c>
       <c r="D18" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="E18" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>375</v>
+      </c>
+      <c r="B19" t="s">
         <v>376</v>
       </c>
-      <c r="B19" t="s">
-        <v>378</v>
-      </c>
       <c r="C19" t="s">
+        <v>379</v>
+      </c>
+      <c r="D19" t="s">
         <v>380</v>
       </c>
-      <c r="D19" t="s">
-        <v>382</v>
-      </c>
       <c r="E19" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B20" t="s">
+        <v>377</v>
+      </c>
+      <c r="C20" t="s">
         <v>379</v>
       </c>
-      <c r="C20" t="s">
-        <v>380</v>
-      </c>
       <c r="D20" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E20" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>298</v>
+        <v>375</v>
       </c>
       <c r="B21" t="s">
-        <v>298</v>
+        <v>378</v>
       </c>
       <c r="C21" t="s">
-        <v>323</v>
+        <v>379</v>
       </c>
       <c r="D21" t="s">
-        <v>341</v>
+        <v>382</v>
       </c>
       <c r="E21" t="s">
-        <v>323</v>
+        <v>385</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B22" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="C22" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D22" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E22" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B23" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D23" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E23" t="s">
-        <v>358</v>
+        <v>324</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1957,55 +1966,55 @@
         <v>300</v>
       </c>
       <c r="B24" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C24" t="s">
         <v>325</v>
       </c>
       <c r="D24" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E24" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B25" t="s">
-        <v>301</v>
+        <v>318</v>
       </c>
       <c r="C25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D25" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="E25" t="s">
-        <v>326</v>
+        <v>359</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>302</v>
+        <v>301</v>
+      </c>
+      <c r="B26" t="s">
+        <v>301</v>
+      </c>
+      <c r="C26" t="s">
+        <v>326</v>
+      </c>
+      <c r="D26" t="s">
+        <v>343</v>
+      </c>
+      <c r="E26" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>303</v>
-      </c>
-      <c r="B27" t="s">
-        <v>319</v>
-      </c>
-      <c r="C27" t="s">
-        <v>366</v>
-      </c>
-      <c r="D27" t="s">
-        <v>346</v>
-      </c>
-      <c r="E27" t="s">
-        <v>360</v>
+        <v>302</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2013,16 +2022,16 @@
         <v>303</v>
       </c>
       <c r="B28" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C28" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D28" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E28" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2030,16 +2039,16 @@
         <v>303</v>
       </c>
       <c r="B29" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C29" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D29" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E29" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2047,16 +2056,33 @@
         <v>303</v>
       </c>
       <c r="B30" t="s">
+        <v>321</v>
+      </c>
+      <c r="C30" t="s">
+        <v>365</v>
+      </c>
+      <c r="D30" t="s">
+        <v>348</v>
+      </c>
+      <c r="E30" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>303</v>
+      </c>
+      <c r="B31" t="s">
+        <v>366</v>
+      </c>
+      <c r="C31" t="s">
+        <v>365</v>
+      </c>
+      <c r="D31" t="s">
         <v>367</v>
       </c>
-      <c r="C30" t="s">
-        <v>366</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="E31" t="s">
         <v>368</v>
-      </c>
-      <c r="E30" t="s">
-        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>